<commit_message>
Patient Base & with Mandatory Idetifier - add must support flag to deceasedDateTime.accuracyIndicator & remove related known issues in PSML; updated PSML mappings
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/medicationstatement-detailed-1.xlsx
+++ b/output/SharedMedicinesList/medicationstatement-detailed-1.xlsx
@@ -557,7 +557,7 @@
     <t>class</t>
   </si>
   <si>
-    <t>MedicationStatement.medicationReference</t>
+    <t>MedicationStatement.medication[x]</t>
   </si>
   <si>
     <t>medicationReference</t>
@@ -574,9 +574,6 @@
   </si>
   <si>
     <t>If only a code is specified, then it needs to be a code for a specific product. If more information is required, then the use of the medication resource is recommended.  For example if you require form or lot number, then you must reference the Medication resource. .</t>
-  </si>
-  <si>
-    <t>MedicationStatement.medication[x]</t>
   </si>
   <si>
     <t>…code</t>
@@ -926,6 +923,9 @@
   </si>
   <si>
     <t>C*E.9. But note many systems use C*E.2 for this</t>
+  </si>
+  <si>
+    <t>MedicationStatement.medicationReference</t>
   </si>
   <si>
     <t xml:space="preserve">Reference(http://hl7.org.au/fhir/StructureDefinition/au-medication)
@@ -4035,28 +4035,28 @@
         <v>40</v>
       </c>
       <c r="AE20" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="AF20" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AG20" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI20" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ20" t="s" s="2">
         <v>174</v>
       </c>
-      <c r="AF20" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AG20" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH20" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI20" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ20" t="s" s="2">
+      <c r="AK20" t="s" s="2">
         <v>175</v>
       </c>
-      <c r="AK20" t="s" s="2">
+      <c r="AL20" t="s" s="2">
         <v>176</v>
-      </c>
-      <c r="AL20" t="s" s="2">
-        <v>177</v>
       </c>
       <c r="AM20" t="s" s="2">
         <v>40</v>
@@ -4064,10 +4064,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="B21" t="s" s="2">
         <v>178</v>
-      </c>
-      <c r="B21" t="s" s="2">
-        <v>179</v>
       </c>
       <c r="C21" t="s" s="2">
         <v>40</v>
@@ -4092,7 +4092,7 @@
         <v>160</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L21" t="s" s="2">
         <v>172</v>
@@ -4124,52 +4124,52 @@
         <v>40</v>
       </c>
       <c r="W21" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="X21" t="s" s="2">
         <v>181</v>
       </c>
-      <c r="X21" t="s" s="2">
+      <c r="Y21" t="s" s="2">
         <v>182</v>
       </c>
-      <c r="Y21" t="s" s="2">
+      <c r="Z21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE21" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="AF21" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AG21" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH21" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI21" t="s" s="2">
         <v>183</v>
       </c>
-      <c r="Z21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE21" t="s" s="2">
+      <c r="AJ21" t="s" s="2">
         <v>174</v>
       </c>
-      <c r="AF21" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AG21" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH21" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI21" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="AJ21" t="s" s="2">
+      <c r="AK21" t="s" s="2">
         <v>175</v>
       </c>
-      <c r="AK21" t="s" s="2">
+      <c r="AL21" t="s" s="2">
         <v>176</v>
-      </c>
-      <c r="AL21" t="s" s="2">
-        <v>177</v>
       </c>
       <c r="AM21" t="s" s="2">
         <v>40</v>
@@ -4177,7 +4177,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -4200,13 +4200,13 @@
         <v>40</v>
       </c>
       <c r="J22" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="K22" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="K22" t="s" s="2">
+      <c r="L22" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="L22" t="s" s="2">
-        <v>188</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -4257,25 +4257,25 @@
         <v>40</v>
       </c>
       <c r="AE22" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AF22" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG22" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ22" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK22" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="AF22" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG22" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ22" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK22" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>40</v>
@@ -4286,7 +4286,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4312,10 +4312,10 @@
         <v>96</v>
       </c>
       <c r="K23" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L23" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="L23" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="M23" t="s" s="2">
         <v>120</v>
@@ -4359,7 +4359,7 @@
         <v>99</v>
       </c>
       <c r="AB23" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC23" t="s" s="2">
         <v>40</v>
@@ -4368,7 +4368,7 @@
         <v>100</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>41</v>
@@ -4386,7 +4386,7 @@
         <v>40</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>40</v>
@@ -4397,7 +4397,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4420,19 +4420,19 @@
         <v>52</v>
       </c>
       <c r="J24" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="K24" t="s" s="2">
         <v>197</v>
       </c>
-      <c r="K24" t="s" s="2">
+      <c r="L24" t="s" s="2">
         <v>198</v>
       </c>
-      <c r="L24" t="s" s="2">
+      <c r="M24" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M24" t="s" s="2">
+      <c r="N24" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>40</v>
@@ -4469,7 +4469,7 @@
         <v>40</v>
       </c>
       <c r="AA24" t="s" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AB24" s="2"/>
       <c r="AC24" t="s" s="2">
@@ -4479,7 +4479,7 @@
         <v>100</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>41</v>
@@ -4497,21 +4497,21 @@
         <v>40</v>
       </c>
       <c r="AK24" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL24" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM24" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL24" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM24" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C25" t="s" s="2">
         <v>40</v>
@@ -4533,19 +4533,19 @@
         <v>52</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K25" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="L25" t="s" s="2">
         <v>207</v>
       </c>
-      <c r="L25" t="s" s="2">
-        <v>208</v>
-      </c>
       <c r="M25" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="N25" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>40</v>
@@ -4574,7 +4574,7 @@
       </c>
       <c r="X25" s="2"/>
       <c r="Y25" t="s" s="2">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>40</v>
@@ -4592,7 +4592,7 @@
         <v>40</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>41</v>
@@ -4610,21 +4610,21 @@
         <v>40</v>
       </c>
       <c r="AK25" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL25" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM25" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL25" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM25" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C26" t="s" s="2">
         <v>40</v>
@@ -4646,19 +4646,19 @@
         <v>52</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K26" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="L26" t="s" s="2">
         <v>211</v>
       </c>
-      <c r="L26" t="s" s="2">
-        <v>212</v>
-      </c>
       <c r="M26" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="N26" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>40</v>
@@ -4687,7 +4687,7 @@
       </c>
       <c r="X26" s="2"/>
       <c r="Y26" t="s" s="2">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>40</v>
@@ -4705,7 +4705,7 @@
         <v>40</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>41</v>
@@ -4723,21 +4723,21 @@
         <v>40</v>
       </c>
       <c r="AK26" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL26" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM26" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL26" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM26" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C27" t="s" s="2">
         <v>40</v>
@@ -4759,19 +4759,19 @@
         <v>52</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L27" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="M27" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M27" t="s" s="2">
+      <c r="N27" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>40</v>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="X27" s="2"/>
       <c r="Y27" t="s" s="2">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>40</v>
@@ -4818,7 +4818,7 @@
         <v>40</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>41</v>
@@ -4836,18 +4836,18 @@
         <v>40</v>
       </c>
       <c r="AK27" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM27" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL27" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM27" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4870,13 +4870,13 @@
         <v>40</v>
       </c>
       <c r="J28" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="K28" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="K28" t="s" s="2">
+      <c r="L28" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="L28" t="s" s="2">
-        <v>188</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -4927,25 +4927,25 @@
         <v>40</v>
       </c>
       <c r="AE28" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AF28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG28" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ28" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK28" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="AF28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG28" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH28" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI28" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ28" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK28" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>40</v>
@@ -4956,7 +4956,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -5027,7 +5027,7 @@
         <v>99</v>
       </c>
       <c r="AB29" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC29" t="s" s="2">
         <v>40</v>
@@ -5036,7 +5036,7 @@
         <v>100</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>41</v>
@@ -5065,10 +5065,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="B30" t="s" s="2">
         <v>218</v>
-      </c>
-      <c r="B30" t="s" s="2">
-        <v>219</v>
       </c>
       <c r="C30" t="s" s="2">
         <v>40</v>
@@ -5090,13 +5090,13 @@
         <v>40</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="K30" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="K30" t="s" s="2">
+      <c r="L30" t="s" s="2">
         <v>221</v>
-      </c>
-      <c r="L30" t="s" s="2">
-        <v>222</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -5147,7 +5147,7 @@
         <v>40</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>41</v>
@@ -5176,7 +5176,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5199,13 +5199,13 @@
         <v>40</v>
       </c>
       <c r="J31" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="K31" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="K31" t="s" s="2">
+      <c r="L31" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="L31" t="s" s="2">
-        <v>188</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -5256,25 +5256,25 @@
         <v>40</v>
       </c>
       <c r="AE31" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AF31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG31" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK31" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="AF31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG31" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH31" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI31" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ31" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK31" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>40</v>
@@ -5285,7 +5285,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5311,10 +5311,10 @@
         <v>96</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="M32" t="s" s="2">
         <v>120</v>
@@ -5358,7 +5358,7 @@
         <v>99</v>
       </c>
       <c r="AB32" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC32" t="s" s="2">
         <v>40</v>
@@ -5367,7 +5367,7 @@
         <v>100</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>41</v>
@@ -5385,7 +5385,7 @@
         <v>40</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>40</v>
@@ -5396,7 +5396,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5422,13 +5422,13 @@
         <v>64</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="L33" t="s" s="2">
         <v>226</v>
       </c>
-      <c r="L33" t="s" s="2">
+      <c r="M33" t="s" s="2">
         <v>227</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>228</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
@@ -5436,49 +5436,49 @@
       </c>
       <c r="P33" s="2"/>
       <c r="Q33" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="R33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD33" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE33" t="s" s="2">
         <v>229</v>
-      </c>
-      <c r="R33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="S33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="T33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE33" t="s" s="2">
-        <v>230</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>51</v>
@@ -5507,10 +5507,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="B34" t="s" s="2">
         <v>231</v>
-      </c>
-      <c r="B34" t="s" s="2">
-        <v>232</v>
       </c>
       <c r="C34" t="s" s="2">
         <v>40</v>
@@ -5532,13 +5532,13 @@
         <v>40</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>233</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>234</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5547,7 +5547,7 @@
       </c>
       <c r="P34" s="2"/>
       <c r="Q34" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="R34" t="s" s="2">
         <v>40</v>
@@ -5568,28 +5568,28 @@
         <v>153</v>
       </c>
       <c r="X34" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="Y34" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="Y34" t="s" s="2">
+      <c r="Z34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD34" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE34" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="Z34" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA34" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB34" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC34" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD34" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE34" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>41</v>
@@ -5618,7 +5618,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5644,16 +5644,16 @@
         <v>64</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>240</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="M35" t="s" s="2">
         <v>241</v>
       </c>
-      <c r="M35" t="s" s="2">
+      <c r="N35" t="s" s="2">
         <v>242</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>243</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>40</v>
@@ -5702,36 +5702,36 @@
         <v>40</v>
       </c>
       <c r="AE35" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="AF35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG35" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK35" t="s" s="2">
         <v>244</v>
       </c>
-      <c r="AF35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG35" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK35" t="s" s="2">
+      <c r="AL35" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM35" t="s" s="2">
         <v>245</v>
-      </c>
-      <c r="AL35" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM35" t="s" s="2">
-        <v>246</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5754,16 +5754,16 @@
         <v>52</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>248</v>
       </c>
-      <c r="L36" t="s" s="2">
+      <c r="M36" t="s" s="2">
         <v>249</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>250</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
@@ -5813,36 +5813,36 @@
         <v>40</v>
       </c>
       <c r="AE36" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="AF36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG36" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK36" t="s" s="2">
         <v>251</v>
       </c>
-      <c r="AF36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG36" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH36" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI36" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ36" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK36" t="s" s="2">
+      <c r="AL36" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM36" t="s" s="2">
         <v>252</v>
-      </c>
-      <c r="AL36" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM36" t="s" s="2">
-        <v>253</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5868,14 +5868,14 @@
         <v>70</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>255</v>
-      </c>
-      <c r="L37" t="s" s="2">
-        <v>256</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" t="s" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>40</v>
@@ -5924,36 +5924,36 @@
         <v>40</v>
       </c>
       <c r="AE37" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="AF37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG37" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH37" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI37" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ37" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK37" t="s" s="2">
         <v>258</v>
       </c>
-      <c r="AF37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG37" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH37" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI37" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ37" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK37" t="s" s="2">
+      <c r="AL37" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM37" t="s" s="2">
         <v>259</v>
-      </c>
-      <c r="AL37" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM37" t="s" s="2">
-        <v>260</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5976,17 +5976,17 @@
         <v>52</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>262</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>263</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" t="s" s="2">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>40</v>
@@ -6035,36 +6035,36 @@
         <v>40</v>
       </c>
       <c r="AE38" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="AF38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG38" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK38" t="s" s="2">
         <v>265</v>
       </c>
-      <c r="AF38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG38" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK38" t="s" s="2">
+      <c r="AL38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM38" t="s" s="2">
         <v>266</v>
-      </c>
-      <c r="AL38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM38" t="s" s="2">
-        <v>267</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6087,19 +6087,19 @@
         <v>52</v>
       </c>
       <c r="J39" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="K39" t="s" s="2">
         <v>269</v>
       </c>
-      <c r="K39" t="s" s="2">
+      <c r="L39" t="s" s="2">
         <v>270</v>
       </c>
-      <c r="L39" t="s" s="2">
+      <c r="M39" t="s" s="2">
         <v>271</v>
       </c>
-      <c r="M39" t="s" s="2">
+      <c r="N39" t="s" s="2">
         <v>272</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>273</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>40</v>
@@ -6148,39 +6148,39 @@
         <v>40</v>
       </c>
       <c r="AE39" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="AF39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG39" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH39" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI39" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ39" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK39" t="s" s="2">
         <v>274</v>
       </c>
-      <c r="AF39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG39" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH39" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI39" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ39" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK39" t="s" s="2">
+      <c r="AL39" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM39" t="s" s="2">
         <v>275</v>
-      </c>
-      <c r="AL39" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM39" t="s" s="2">
-        <v>276</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C40" t="s" s="2">
         <v>40</v>
@@ -6202,19 +6202,19 @@
         <v>52</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L40" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="M40" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M40" t="s" s="2">
+      <c r="N40" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>40</v>
@@ -6243,7 +6243,7 @@
       </c>
       <c r="X40" s="2"/>
       <c r="Y40" t="s" s="2">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>40</v>
@@ -6261,7 +6261,7 @@
         <v>40</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>41</v>
@@ -6279,18 +6279,18 @@
         <v>40</v>
       </c>
       <c r="AK40" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL40" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM40" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL40" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM40" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6313,19 +6313,19 @@
         <v>52</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="M41" t="s" s="2">
+      <c r="N41" t="s" s="2">
         <v>283</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>40</v>
@@ -6374,36 +6374,36 @@
         <v>40</v>
       </c>
       <c r="AE41" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AF41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG41" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK41" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="AF41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG41" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK41" t="s" s="2">
+      <c r="AL41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM41" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="AL41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM41" t="s" s="2">
-        <v>287</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>168</v>
+        <v>287</v>
       </c>
       <c r="B42" t="s" s="2">
         <v>169</v>
@@ -6487,28 +6487,28 @@
         <v>40</v>
       </c>
       <c r="AE42" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="AF42" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AG42" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH42" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI42" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ42" t="s" s="2">
         <v>174</v>
       </c>
-      <c r="AF42" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AG42" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH42" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI42" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ42" t="s" s="2">
+      <c r="AK42" t="s" s="2">
         <v>175</v>
       </c>
-      <c r="AK42" t="s" s="2">
+      <c r="AL42" t="s" s="2">
         <v>176</v>
-      </c>
-      <c r="AL42" t="s" s="2">
-        <v>177</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>40</v>
@@ -7232,7 +7232,7 @@
         <v>40</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="X49" t="s" s="2">
         <v>336</v>
@@ -7308,13 +7308,13 @@
         <v>40</v>
       </c>
       <c r="J50" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="K50" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="K50" t="s" s="2">
+      <c r="L50" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>188</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -7365,25 +7365,25 @@
         <v>40</v>
       </c>
       <c r="AE50" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AF50" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG50" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ50" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK50" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="AF50" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG50" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ50" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK50" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>40</v>
@@ -7420,10 +7420,10 @@
         <v>96</v>
       </c>
       <c r="K51" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="M51" t="s" s="2">
         <v>120</v>
@@ -7467,7 +7467,7 @@
         <v>99</v>
       </c>
       <c r="AB51" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC51" t="s" s="2">
         <v>40</v>
@@ -7476,7 +7476,7 @@
         <v>100</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
@@ -7494,7 +7494,7 @@
         <v>40</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>40</v>
@@ -7528,19 +7528,19 @@
         <v>52</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K52" t="s" s="2">
         <v>343</v>
       </c>
       <c r="L52" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="M52" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M52" t="s" s="2">
+      <c r="N52" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>40</v>
@@ -7587,7 +7587,7 @@
         <v>100</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
@@ -7605,13 +7605,13 @@
         <v>40</v>
       </c>
       <c r="AK52" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM52" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM52" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="53" hidden="true">
@@ -7641,19 +7641,19 @@
         <v>52</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K53" t="s" s="2">
         <v>346</v>
       </c>
       <c r="L53" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="M53" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M53" t="s" s="2">
+      <c r="N53" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N53" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>40</v>
@@ -7700,7 +7700,7 @@
         <v>40</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>41</v>
@@ -7718,13 +7718,13 @@
         <v>40</v>
       </c>
       <c r="AK53" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM53" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM53" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="54" hidden="true">
@@ -7752,19 +7752,19 @@
         <v>52</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K54" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="L54" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="L54" t="s" s="2">
+      <c r="M54" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="M54" t="s" s="2">
+      <c r="N54" t="s" s="2">
         <v>283</v>
-      </c>
-      <c r="N54" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>40</v>
@@ -7813,31 +7813,31 @@
         <v>40</v>
       </c>
       <c r="AE54" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK54" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="AF54" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG54" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK54" t="s" s="2">
+      <c r="AL54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM54" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="AL54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM54" t="s" s="2">
-        <v>287</v>
       </c>
     </row>
     <row r="55">
@@ -7900,7 +7900,7 @@
         <v>40</v>
       </c>
       <c r="W55" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="X55" t="s" s="2">
         <v>353</v>
@@ -7976,13 +7976,13 @@
         <v>40</v>
       </c>
       <c r="J56" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="K56" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="K56" t="s" s="2">
+      <c r="L56" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="L56" t="s" s="2">
-        <v>188</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -8033,25 +8033,25 @@
         <v>40</v>
       </c>
       <c r="AE56" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AF56" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG56" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ56" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK56" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="AF56" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG56" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH56" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI56" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ56" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK56" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>40</v>
@@ -8088,10 +8088,10 @@
         <v>96</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L57" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="L57" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="M57" t="s" s="2">
         <v>120</v>
@@ -8135,7 +8135,7 @@
         <v>99</v>
       </c>
       <c r="AB57" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC57" t="s" s="2">
         <v>40</v>
@@ -8144,7 +8144,7 @@
         <v>100</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
@@ -8162,7 +8162,7 @@
         <v>40</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>40</v>
@@ -8196,19 +8196,19 @@
         <v>52</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K58" t="s" s="2">
         <v>343</v>
       </c>
       <c r="L58" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="M58" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M58" t="s" s="2">
+      <c r="N58" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>40</v>
@@ -8255,7 +8255,7 @@
         <v>100</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
@@ -8273,13 +8273,13 @@
         <v>40</v>
       </c>
       <c r="AK58" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL58" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM58" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL58" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM58" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="59" hidden="true">
@@ -8309,19 +8309,19 @@
         <v>52</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K59" t="s" s="2">
         <v>362</v>
       </c>
       <c r="L59" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="M59" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M59" t="s" s="2">
+      <c r="N59" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>40</v>
@@ -8368,7 +8368,7 @@
         <v>40</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
@@ -8386,13 +8386,13 @@
         <v>40</v>
       </c>
       <c r="AK59" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL59" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM59" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL59" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM59" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="60" hidden="true">
@@ -8420,19 +8420,19 @@
         <v>52</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="L60" t="s" s="2">
+      <c r="M60" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="M60" t="s" s="2">
+      <c r="N60" t="s" s="2">
         <v>283</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>40</v>
@@ -8481,31 +8481,31 @@
         <v>40</v>
       </c>
       <c r="AE60" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AF60" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG60" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK60" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="AF60" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG60" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH60" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI60" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ60" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK60" t="s" s="2">
+      <c r="AL60" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM60" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="AL60" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM60" t="s" s="2">
-        <v>287</v>
       </c>
     </row>
     <row r="61" hidden="true">
@@ -8864,13 +8864,13 @@
         <v>40</v>
       </c>
       <c r="J64" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="K64" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="K64" t="s" s="2">
+      <c r="L64" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="L64" t="s" s="2">
-        <v>188</v>
       </c>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
@@ -8921,25 +8921,25 @@
         <v>40</v>
       </c>
       <c r="AE64" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AF64" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG64" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH64" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI64" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ64" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK64" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="AF64" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG64" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH64" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI64" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ64" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK64" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>40</v>
@@ -8976,10 +8976,10 @@
         <v>96</v>
       </c>
       <c r="K65" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L65" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="L65" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="M65" t="s" s="2">
         <v>120</v>
@@ -9023,7 +9023,7 @@
         <v>99</v>
       </c>
       <c r="AB65" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC65" t="s" s="2">
         <v>40</v>
@@ -9032,7 +9032,7 @@
         <v>100</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
@@ -9050,7 +9050,7 @@
         <v>40</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>40</v>
@@ -9195,7 +9195,7 @@
         <v>52</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K67" t="s" s="2">
         <v>395</v>
@@ -9341,7 +9341,7 @@
         <v>40</v>
       </c>
       <c r="W68" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="X68" t="s" s="2">
         <v>403</v>
@@ -9526,7 +9526,7 @@
         <v>52</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K70" t="s" s="2">
         <v>410</v>
@@ -9783,7 +9783,7 @@
         <v>40</v>
       </c>
       <c r="W72" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="X72" t="s" s="2">
         <v>425</v>
@@ -9896,7 +9896,7 @@
         <v>40</v>
       </c>
       <c r="W73" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="X73" t="s" s="2">
         <v>425</v>
@@ -9972,13 +9972,13 @@
         <v>40</v>
       </c>
       <c r="J74" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="K74" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="K74" t="s" s="2">
+      <c r="L74" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="L74" t="s" s="2">
-        <v>188</v>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -10029,25 +10029,25 @@
         <v>40</v>
       </c>
       <c r="AE74" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AF74" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG74" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH74" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI74" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ74" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK74" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="AF74" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG74" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK74" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="AL74" t="s" s="2">
         <v>40</v>
@@ -10084,10 +10084,10 @@
         <v>96</v>
       </c>
       <c r="K75" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L75" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="L75" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="M75" t="s" s="2">
         <v>120</v>
@@ -10131,7 +10131,7 @@
         <v>99</v>
       </c>
       <c r="AB75" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC75" t="s" s="2">
         <v>40</v>
@@ -10154,7 +10154,7 @@
         <v>40</v>
       </c>
       <c r="AK75" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AL75" t="s" s="2">
         <v>40</v>
@@ -10225,7 +10225,7 @@
         <v>40</v>
       </c>
       <c r="W76" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="X76" t="s" s="2">
         <v>425</v>
@@ -10301,13 +10301,13 @@
         <v>40</v>
       </c>
       <c r="J77" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="K77" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="K77" t="s" s="2">
+      <c r="L77" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="L77" t="s" s="2">
-        <v>188</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -10358,25 +10358,25 @@
         <v>40</v>
       </c>
       <c r="AE77" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AF77" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG77" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH77" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI77" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ77" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK77" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="AF77" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG77" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ77" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK77" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="AL77" t="s" s="2">
         <v>40</v>
@@ -10413,10 +10413,10 @@
         <v>96</v>
       </c>
       <c r="K78" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L78" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="L78" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="M78" t="s" s="2">
         <v>120</v>
@@ -10460,7 +10460,7 @@
         <v>99</v>
       </c>
       <c r="AB78" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC78" t="s" s="2">
         <v>40</v>
@@ -10469,7 +10469,7 @@
         <v>100</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>41</v>
@@ -10487,7 +10487,7 @@
         <v>40</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>40</v>
@@ -10521,19 +10521,19 @@
         <v>52</v>
       </c>
       <c r="J79" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K79" t="s" s="2">
         <v>343</v>
       </c>
       <c r="L79" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="M79" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M79" t="s" s="2">
+      <c r="N79" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N79" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O79" t="s" s="2">
         <v>40</v>
@@ -10580,7 +10580,7 @@
         <v>100</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>41</v>
@@ -10598,13 +10598,13 @@
         <v>40</v>
       </c>
       <c r="AK79" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL79" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM79" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL79" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM79" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="80" hidden="true">
@@ -10634,19 +10634,19 @@
         <v>52</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K80" t="s" s="2">
         <v>438</v>
       </c>
       <c r="L80" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="M80" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M80" t="s" s="2">
+      <c r="N80" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N80" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O80" t="s" s="2">
         <v>40</v>
@@ -10693,7 +10693,7 @@
         <v>40</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>41</v>
@@ -10711,13 +10711,13 @@
         <v>40</v>
       </c>
       <c r="AK80" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL80" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM80" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL80" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM80" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="81" hidden="true">
@@ -10745,19 +10745,19 @@
         <v>52</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K81" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="L81" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="L81" t="s" s="2">
+      <c r="M81" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="M81" t="s" s="2">
+      <c r="N81" t="s" s="2">
         <v>283</v>
-      </c>
-      <c r="N81" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="O81" t="s" s="2">
         <v>40</v>
@@ -10806,31 +10806,31 @@
         <v>40</v>
       </c>
       <c r="AE81" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AF81" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG81" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK81" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="AF81" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG81" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK81" t="s" s="2">
+      <c r="AL81" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM81" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="AL81" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM81" t="s" s="2">
-        <v>287</v>
       </c>
     </row>
     <row r="82" hidden="true">
@@ -10895,7 +10895,7 @@
         <v>40</v>
       </c>
       <c r="W82" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="X82" t="s" s="2">
         <v>446</v>
@@ -10971,13 +10971,13 @@
         <v>40</v>
       </c>
       <c r="J83" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="K83" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="K83" t="s" s="2">
+      <c r="L83" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="L83" t="s" s="2">
-        <v>188</v>
       </c>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -11028,25 +11028,25 @@
         <v>40</v>
       </c>
       <c r="AE83" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AF83" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG83" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ83" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK83" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="AF83" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG83" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ83" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK83" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="AL83" t="s" s="2">
         <v>40</v>
@@ -11083,10 +11083,10 @@
         <v>96</v>
       </c>
       <c r="K84" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L84" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="L84" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="M84" t="s" s="2">
         <v>120</v>
@@ -11130,7 +11130,7 @@
         <v>99</v>
       </c>
       <c r="AB84" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC84" t="s" s="2">
         <v>40</v>
@@ -11139,7 +11139,7 @@
         <v>100</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>41</v>
@@ -11157,7 +11157,7 @@
         <v>40</v>
       </c>
       <c r="AK84" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AL84" t="s" s="2">
         <v>40</v>
@@ -11191,19 +11191,19 @@
         <v>52</v>
       </c>
       <c r="J85" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K85" t="s" s="2">
         <v>343</v>
       </c>
       <c r="L85" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="M85" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M85" t="s" s="2">
+      <c r="N85" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N85" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O85" t="s" s="2">
         <v>40</v>
@@ -11250,7 +11250,7 @@
         <v>40</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>41</v>
@@ -11268,13 +11268,13 @@
         <v>40</v>
       </c>
       <c r="AK85" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL85" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM85" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL85" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM85" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="86" hidden="true">
@@ -11302,19 +11302,19 @@
         <v>52</v>
       </c>
       <c r="J86" t="s" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K86" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="L86" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="L86" t="s" s="2">
+      <c r="M86" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="M86" t="s" s="2">
+      <c r="N86" t="s" s="2">
         <v>283</v>
-      </c>
-      <c r="N86" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="O86" t="s" s="2">
         <v>40</v>
@@ -11363,31 +11363,31 @@
         <v>40</v>
       </c>
       <c r="AE86" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AF86" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG86" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK86" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="AF86" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG86" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK86" t="s" s="2">
+      <c r="AL86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM86" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="AL86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM86" t="s" s="2">
-        <v>287</v>
       </c>
     </row>
     <row r="87" hidden="true">
@@ -11450,7 +11450,7 @@
         <v>40</v>
       </c>
       <c r="W87" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="X87" t="s" s="2">
         <v>459</v>
@@ -11526,13 +11526,13 @@
         <v>40</v>
       </c>
       <c r="J88" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="K88" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="K88" t="s" s="2">
+      <c r="L88" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="L88" t="s" s="2">
-        <v>188</v>
       </c>
       <c r="M88" s="2"/>
       <c r="N88" s="2"/>
@@ -11583,25 +11583,25 @@
         <v>40</v>
       </c>
       <c r="AE88" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AF88" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG88" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ88" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK88" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="AF88" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG88" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH88" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI88" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ88" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK88" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="AL88" t="s" s="2">
         <v>40</v>
@@ -11638,10 +11638,10 @@
         <v>96</v>
       </c>
       <c r="K89" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L89" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="L89" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="M89" t="s" s="2">
         <v>120</v>
@@ -11685,7 +11685,7 @@
         <v>99</v>
       </c>
       <c r="AB89" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC89" t="s" s="2">
         <v>40</v>
@@ -11694,7 +11694,7 @@
         <v>100</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>41</v>
@@ -11712,7 +11712,7 @@
         <v>40</v>
       </c>
       <c r="AK89" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AL89" t="s" s="2">
         <v>40</v>
@@ -11746,19 +11746,19 @@
         <v>52</v>
       </c>
       <c r="J90" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K90" t="s" s="2">
         <v>343</v>
       </c>
       <c r="L90" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="M90" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M90" t="s" s="2">
+      <c r="N90" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N90" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O90" t="s" s="2">
         <v>40</v>
@@ -11805,7 +11805,7 @@
         <v>100</v>
       </c>
       <c r="AE90" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF90" t="s" s="2">
         <v>41</v>
@@ -11823,13 +11823,13 @@
         <v>40</v>
       </c>
       <c r="AK90" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL90" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM90" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL90" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM90" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="91" hidden="true">
@@ -11857,19 +11857,19 @@
         <v>52</v>
       </c>
       <c r="J91" t="s" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K91" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="L91" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="L91" t="s" s="2">
+      <c r="M91" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="M91" t="s" s="2">
+      <c r="N91" t="s" s="2">
         <v>283</v>
-      </c>
-      <c r="N91" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="O91" t="s" s="2">
         <v>40</v>
@@ -11918,31 +11918,31 @@
         <v>40</v>
       </c>
       <c r="AE91" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AF91" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG91" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK91" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="AF91" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG91" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH91" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI91" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ91" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK91" t="s" s="2">
+      <c r="AL91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM91" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="AL91" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM91" t="s" s="2">
-        <v>287</v>
       </c>
     </row>
     <row r="92" hidden="true">
@@ -11970,13 +11970,13 @@
         <v>40</v>
       </c>
       <c r="J92" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="K92" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="K92" t="s" s="2">
+      <c r="L92" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="L92" t="s" s="2">
-        <v>188</v>
       </c>
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
@@ -12027,25 +12027,25 @@
         <v>40</v>
       </c>
       <c r="AE92" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AF92" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG92" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK92" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="AF92" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG92" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH92" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI92" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ92" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK92" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="AL92" t="s" s="2">
         <v>40</v>
@@ -12082,10 +12082,10 @@
         <v>96</v>
       </c>
       <c r="K93" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L93" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="L93" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="M93" t="s" s="2">
         <v>120</v>
@@ -12129,7 +12129,7 @@
         <v>99</v>
       </c>
       <c r="AB93" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC93" t="s" s="2">
         <v>40</v>
@@ -12138,7 +12138,7 @@
         <v>100</v>
       </c>
       <c r="AE93" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF93" t="s" s="2">
         <v>41</v>
@@ -12156,7 +12156,7 @@
         <v>40</v>
       </c>
       <c r="AK93" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AL93" t="s" s="2">
         <v>40</v>
@@ -12190,19 +12190,19 @@
         <v>52</v>
       </c>
       <c r="J94" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K94" t="s" s="2">
         <v>343</v>
       </c>
       <c r="L94" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="M94" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M94" t="s" s="2">
+      <c r="N94" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N94" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O94" t="s" s="2">
         <v>40</v>
@@ -12249,7 +12249,7 @@
         <v>100</v>
       </c>
       <c r="AE94" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF94" t="s" s="2">
         <v>41</v>
@@ -12267,13 +12267,13 @@
         <v>40</v>
       </c>
       <c r="AK94" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL94" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM94" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL94" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM94" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="95" hidden="true">
@@ -12303,19 +12303,19 @@
         <v>52</v>
       </c>
       <c r="J95" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K95" t="s" s="2">
         <v>468</v>
       </c>
       <c r="L95" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="M95" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M95" t="s" s="2">
+      <c r="N95" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N95" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O95" t="s" s="2">
         <v>40</v>
@@ -12362,7 +12362,7 @@
         <v>40</v>
       </c>
       <c r="AE95" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF95" t="s" s="2">
         <v>41</v>
@@ -12380,13 +12380,13 @@
         <v>40</v>
       </c>
       <c r="AK95" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL95" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM95" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL95" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM95" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="96" hidden="true">
@@ -12414,19 +12414,19 @@
         <v>52</v>
       </c>
       <c r="J96" t="s" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K96" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="L96" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="L96" t="s" s="2">
+      <c r="M96" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="M96" t="s" s="2">
+      <c r="N96" t="s" s="2">
         <v>283</v>
-      </c>
-      <c r="N96" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="O96" t="s" s="2">
         <v>40</v>
@@ -12475,31 +12475,31 @@
         <v>40</v>
       </c>
       <c r="AE96" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AF96" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG96" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK96" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="AF96" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG96" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH96" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI96" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ96" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK96" t="s" s="2">
+      <c r="AL96" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM96" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="AL96" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM96" t="s" s="2">
-        <v>287</v>
       </c>
     </row>
     <row r="97" hidden="true">
@@ -12564,7 +12564,7 @@
         <v>40</v>
       </c>
       <c r="W97" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="X97" t="s" s="2">
         <v>475</v>
@@ -12640,13 +12640,13 @@
         <v>40</v>
       </c>
       <c r="J98" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="K98" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="K98" t="s" s="2">
+      <c r="L98" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="L98" t="s" s="2">
-        <v>188</v>
       </c>
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
@@ -12697,25 +12697,25 @@
         <v>40</v>
       </c>
       <c r="AE98" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AF98" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG98" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ98" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK98" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="AF98" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG98" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH98" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI98" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ98" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK98" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="AL98" t="s" s="2">
         <v>40</v>
@@ -12752,10 +12752,10 @@
         <v>96</v>
       </c>
       <c r="K99" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L99" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="L99" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="M99" t="s" s="2">
         <v>120</v>
@@ -12799,7 +12799,7 @@
         <v>99</v>
       </c>
       <c r="AB99" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC99" t="s" s="2">
         <v>40</v>
@@ -12808,7 +12808,7 @@
         <v>100</v>
       </c>
       <c r="AE99" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF99" t="s" s="2">
         <v>41</v>
@@ -12826,7 +12826,7 @@
         <v>40</v>
       </c>
       <c r="AK99" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AL99" t="s" s="2">
         <v>40</v>
@@ -12860,19 +12860,19 @@
         <v>52</v>
       </c>
       <c r="J100" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K100" t="s" s="2">
         <v>343</v>
       </c>
       <c r="L100" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="M100" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M100" t="s" s="2">
+      <c r="N100" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N100" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O100" t="s" s="2">
         <v>40</v>
@@ -12919,7 +12919,7 @@
         <v>100</v>
       </c>
       <c r="AE100" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF100" t="s" s="2">
         <v>41</v>
@@ -12937,13 +12937,13 @@
         <v>40</v>
       </c>
       <c r="AK100" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL100" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM100" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL100" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM100" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="101" hidden="true">
@@ -12971,19 +12971,19 @@
         <v>52</v>
       </c>
       <c r="J101" t="s" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K101" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="L101" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="L101" t="s" s="2">
+      <c r="M101" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="M101" t="s" s="2">
+      <c r="N101" t="s" s="2">
         <v>283</v>
-      </c>
-      <c r="N101" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="O101" t="s" s="2">
         <v>40</v>
@@ -13032,31 +13032,31 @@
         <v>40</v>
       </c>
       <c r="AE101" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AF101" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG101" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH101" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI101" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ101" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK101" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="AF101" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG101" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH101" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI101" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ101" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK101" t="s" s="2">
+      <c r="AL101" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM101" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="AL101" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM101" t="s" s="2">
-        <v>287</v>
       </c>
     </row>
     <row r="102" hidden="true">
@@ -13084,13 +13084,13 @@
         <v>40</v>
       </c>
       <c r="J102" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="K102" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="K102" t="s" s="2">
+      <c r="L102" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="L102" t="s" s="2">
-        <v>188</v>
       </c>
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
@@ -13141,25 +13141,25 @@
         <v>40</v>
       </c>
       <c r="AE102" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AF102" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG102" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH102" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI102" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ102" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK102" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="AF102" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG102" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH102" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI102" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ102" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK102" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="AL102" t="s" s="2">
         <v>40</v>
@@ -13196,10 +13196,10 @@
         <v>96</v>
       </c>
       <c r="K103" t="s" s="2">
+        <v>191</v>
+      </c>
+      <c r="L103" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="L103" t="s" s="2">
-        <v>193</v>
       </c>
       <c r="M103" t="s" s="2">
         <v>120</v>
@@ -13243,7 +13243,7 @@
         <v>99</v>
       </c>
       <c r="AB103" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC103" t="s" s="2">
         <v>40</v>
@@ -13252,7 +13252,7 @@
         <v>100</v>
       </c>
       <c r="AE103" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AF103" t="s" s="2">
         <v>41</v>
@@ -13270,7 +13270,7 @@
         <v>40</v>
       </c>
       <c r="AK103" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AL103" t="s" s="2">
         <v>40</v>
@@ -13304,19 +13304,19 @@
         <v>52</v>
       </c>
       <c r="J104" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K104" t="s" s="2">
         <v>343</v>
       </c>
       <c r="L104" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="M104" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M104" t="s" s="2">
+      <c r="N104" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N104" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O104" t="s" s="2">
         <v>40</v>
@@ -13363,7 +13363,7 @@
         <v>100</v>
       </c>
       <c r="AE104" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF104" t="s" s="2">
         <v>41</v>
@@ -13381,13 +13381,13 @@
         <v>40</v>
       </c>
       <c r="AK104" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL104" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM104" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL104" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM104" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="105" hidden="true">
@@ -13417,19 +13417,19 @@
         <v>52</v>
       </c>
       <c r="J105" t="s" s="2">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K105" t="s" s="2">
         <v>484</v>
       </c>
       <c r="L105" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="M105" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="M105" t="s" s="2">
+      <c r="N105" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="N105" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="O105" t="s" s="2">
         <v>40</v>
@@ -13476,7 +13476,7 @@
         <v>40</v>
       </c>
       <c r="AE105" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF105" t="s" s="2">
         <v>41</v>
@@ -13494,13 +13494,13 @@
         <v>40</v>
       </c>
       <c r="AK105" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="AL105" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM105" t="s" s="2">
         <v>204</v>
-      </c>
-      <c r="AL105" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM105" t="s" s="2">
-        <v>205</v>
       </c>
     </row>
     <row r="106" hidden="true">
@@ -13528,19 +13528,19 @@
         <v>52</v>
       </c>
       <c r="J106" t="s" s="2">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K106" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="L106" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="L106" t="s" s="2">
+      <c r="M106" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="M106" t="s" s="2">
+      <c r="N106" t="s" s="2">
         <v>283</v>
-      </c>
-      <c r="N106" t="s" s="2">
-        <v>284</v>
       </c>
       <c r="O106" t="s" s="2">
         <v>40</v>
@@ -13589,31 +13589,31 @@
         <v>40</v>
       </c>
       <c r="AE106" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AF106" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG106" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH106" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI106" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ106" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK106" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="AF106" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG106" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH106" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI106" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ106" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK106" t="s" s="2">
+      <c r="AL106" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM106" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="AL106" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM106" t="s" s="2">
-        <v>287</v>
       </c>
     </row>
     <row r="107" hidden="true">

</xml_diff>

<commit_message>
Regenerated SML outputs - updated dosage constraints in medicationstatement-detailed-1
- relaxed the dosage constraint from 1..* to 0..*
- added invariant to ensure that if the status is active or intended, then dosage shall be provided

Github: #76
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/medicationstatement-detailed-1.xlsx
+++ b/output/SharedMedicinesList/medicationstatement-detailed-1.xlsx
@@ -167,7 +167,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}mst-1:Reason not taken is only permitted if Taken is No {reasonNotTaken.exists().not() or (taken = 'n')}inv-dh-mst-02:If present, an information source shall at least have a reference, an identifier or a display {informationSource.exists() implies informationSource.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}inv-dh-mst-03:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}mst-1:Reason not taken is only permitted if Taken is No {reasonNotTaken.exists().not() or (taken = 'n')}inv-dh-mst-02:If present, an information source shall at least have a reference, an identifier or a display {informationSource.exists() implies informationSource.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}inv-dh-mst-03:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-mst-04:If status is active or intended, then dosage shall be provided {(status='active' or status='intended') implies dosage.exists()}</t>
   </si>
   <si>
     <t>..Event</t>
@@ -10165,7 +10165,7 @@
       </c>
       <c r="D80" s="2"/>
       <c r="E80" t="s" s="2">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F80" t="s" s="2">
         <v>42</v>

</xml_diff>